<commit_message>
Add data for chapter 8
</commit_message>
<xml_diff>
--- a/data/java-issues-quantitative-results.xlsx
+++ b/data/java-issues-quantitative-results.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31200" windowHeight="18780" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31200" windowHeight="18780" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data for all bm" sheetId="2" r:id="rId1"/>
+    <sheet name="Data for all bm (2)" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>Support for constant data</t>
   </si>
@@ -121,12 +122,27 @@
   </si>
   <si>
     <t>Size of constant data</t>
+  </si>
+  <si>
+    <t>Support for nested data structures</t>
+  </si>
+  <si>
+    <t>Size of main data structures in C</t>
+  </si>
+  <si>
+    <t>Size of main data structures in Java</t>
+  </si>
+  <si>
+    <t>Size increase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -191,7 +207,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -265,10 +281,55 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -276,9 +337,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="119">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -315,6 +383,29 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -351,6 +442,29 @@
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -682,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -740,10 +854,10 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C4">
@@ -787,8 +901,8 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C5">
@@ -809,7 +923,7 @@
       <c r="H5">
         <v>208</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>2056</v>
       </c>
       <c r="J5">
@@ -821,7 +935,7 @@
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="M5" s="5" t="s">
         <v>27</v>
       </c>
       <c r="N5">
@@ -832,8 +946,8 @@
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C6">
@@ -854,7 +968,7 @@
       <c r="H6">
         <v>1998</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="10">
         <v>26714</v>
       </c>
       <c r="J6">
@@ -866,7 +980,7 @@
       <c r="L6">
         <v>0</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="M6" s="5" t="s">
         <v>27</v>
       </c>
       <c r="N6">
@@ -877,10 +991,10 @@
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C7">
@@ -924,8 +1038,8 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C8">
@@ -969,245 +1083,245 @@
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <f>100*C7/C8</f>
         <v>9.0909090909090917</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <f t="shared" ref="D9:P9" si="0">100*D7/D8</f>
         <v>25</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <f t="shared" si="0"/>
         <v>31.25</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <f t="shared" si="0"/>
         <v>21.05263157894737</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="11">
         <f t="shared" si="0"/>
         <v>4.8484848484848486</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <f t="shared" si="0"/>
         <v>29.62962962962963</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <f>100*I7/I8</f>
         <v>21.917808219178081</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="6">
         <f>100*J7/J8</f>
         <v>6.9767441860465116</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="6">
         <f>100*K7/K8</f>
         <v>16.666666666666668</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="6">
         <f>100*L7/L8</f>
         <v>6.4364207221350078</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="6">
         <f>100*M7/M8</f>
         <v>6.9473684210526319</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N9" s="6">
         <f>100*N7/N8</f>
         <v>8.5106382978723403</v>
       </c>
-      <c r="O9" s="8">
+      <c r="O9" s="7">
         <f>100*O7/O8</f>
         <v>25.735294117647058</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="5" customFormat="1">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:15" s="4" customFormat="1">
+      <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
-      <c r="D10" s="6">
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
         <v>1.69</v>
       </c>
-      <c r="E10" s="5">
-        <v>1</v>
-      </c>
-      <c r="F10" s="6">
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5">
         <v>1.57</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>1.25</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>1.37</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>1.2</v>
       </c>
-      <c r="J10" s="5">
-        <v>1</v>
-      </c>
-      <c r="K10" s="5">
-        <v>1</v>
-      </c>
-      <c r="L10" s="5">
+      <c r="J10" s="4">
+        <v>1</v>
+      </c>
+      <c r="K10" s="4">
+        <v>1</v>
+      </c>
+      <c r="L10" s="4">
         <v>1.08</v>
       </c>
-      <c r="M10" s="5">
-        <v>1</v>
-      </c>
-      <c r="N10" s="5">
-        <v>1</v>
-      </c>
-      <c r="O10" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" s="5" customFormat="1">
-      <c r="B11" s="5" t="s">
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
+      <c r="N10" s="4">
+        <v>1</v>
+      </c>
+      <c r="O10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="4" customFormat="1">
+      <c r="B11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="5">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
         <v>42</v>
       </c>
-      <c r="E11" s="5">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5">
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
         <v>-224</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>-1502</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>-94</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <v>-20</v>
       </c>
-      <c r="J11" s="5">
-        <v>0</v>
-      </c>
-      <c r="K11" s="5">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6">
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5">
         <v>48</v>
       </c>
-      <c r="M11" s="5">
-        <v>0</v>
-      </c>
-      <c r="N11" s="5">
-        <v>0</v>
-      </c>
-      <c r="O11" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" s="5" customFormat="1">
-      <c r="A12" s="5" t="s">
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="4" customFormat="1">
+      <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>1.91</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>1.52</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>6.44</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>1.03</v>
       </c>
-      <c r="G12" s="5">
-        <v>1</v>
-      </c>
-      <c r="H12" s="5">
-        <v>1</v>
-      </c>
-      <c r="I12" s="5">
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4">
         <v>1.03</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="4">
         <v>1.23</v>
       </c>
-      <c r="K12" s="5">
-        <v>1</v>
-      </c>
-      <c r="L12" s="6">
+      <c r="K12" s="4">
+        <v>1</v>
+      </c>
+      <c r="L12" s="5">
         <v>2.16</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="5">
         <v>1.76</v>
       </c>
-      <c r="N12" s="5">
-        <v>1</v>
-      </c>
-      <c r="O12" s="5">
+      <c r="N12" s="4">
+        <v>1</v>
+      </c>
+      <c r="O12" s="4">
         <v>1.02</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="5" customFormat="1">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:15" s="4" customFormat="1">
+      <c r="A13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="5">
-        <v>1</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1</v>
-      </c>
-      <c r="E13" s="5">
-        <v>1</v>
-      </c>
-      <c r="F13" s="5">
-        <v>1</v>
-      </c>
-      <c r="G13" s="5">
-        <v>1</v>
-      </c>
-      <c r="H13" s="5">
-        <v>1</v>
-      </c>
-      <c r="I13" s="5">
-        <v>1</v>
-      </c>
-      <c r="J13" s="5">
-        <v>1</v>
-      </c>
-      <c r="K13" s="6">
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4">
+        <v>1</v>
+      </c>
+      <c r="I13" s="4">
+        <v>1</v>
+      </c>
+      <c r="J13" s="4">
+        <v>1</v>
+      </c>
+      <c r="K13" s="5">
         <v>4.3</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="4">
         <v>1.06</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="5">
         <v>1.65</v>
       </c>
-      <c r="N13" s="5">
-        <v>1</v>
-      </c>
-      <c r="O13" s="5">
+      <c r="N13" s="4">
+        <v>1</v>
+      </c>
+      <c r="O13" s="4">
         <v>1</v>
       </c>
     </row>
@@ -1216,8 +1330,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="4" customFormat="1">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:15" s="3" customFormat="1">
+      <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1586,55 +1700,55 @@
         <f t="shared" si="4"/>
         <v>Casts per 100 LOC</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
         <f t="shared" si="4"/>
         <v>9.0909090909090917</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="6">
         <f t="shared" ref="D24:O24" si="8">D9</f>
         <v>25</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <f t="shared" si="8"/>
         <v>31.25</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="6">
         <f t="shared" si="8"/>
         <v>21.05263157894737</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="6">
         <f t="shared" si="8"/>
         <v>4.8484848484848486</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="6">
         <f t="shared" si="8"/>
         <v>29.62962962962963</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="6">
         <f t="shared" si="8"/>
         <v>21.917808219178081</v>
       </c>
-      <c r="J24" s="7">
+      <c r="J24" s="6">
         <f t="shared" si="8"/>
         <v>6.9767441860465116</v>
       </c>
-      <c r="K24" s="7">
+      <c r="K24" s="6">
         <f t="shared" si="8"/>
         <v>16.666666666666668</v>
       </c>
-      <c r="L24" s="7">
+      <c r="L24" s="6">
         <f t="shared" si="8"/>
         <v>6.4364207221350078</v>
       </c>
-      <c r="M24" s="7">
+      <c r="M24" s="6">
         <f t="shared" si="8"/>
         <v>6.9473684210526319</v>
       </c>
-      <c r="N24" s="7">
+      <c r="N24" s="6">
         <f t="shared" si="8"/>
         <v>8.5106382978723403</v>
       </c>
-      <c r="O24" s="7">
+      <c r="O24" s="6">
         <f t="shared" si="8"/>
         <v>25.735294117647058</v>
       </c>
@@ -1884,15 +1998,1550 @@
       </c>
     </row>
     <row r="36" spans="5:13">
-      <c r="E36" s="2"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:P36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="4"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>200</v>
+      </c>
+      <c r="I4" s="4">
+        <v>2048</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <v>51</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0</v>
+      </c>
+      <c r="P4" s="4"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>208</v>
+      </c>
+      <c r="I5" s="4">
+        <v>2056</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <v>67</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0</v>
+      </c>
+      <c r="O5" s="4">
+        <v>0</v>
+      </c>
+      <c r="P5" s="4"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1998</v>
+      </c>
+      <c r="I6" s="14">
+        <v>26714</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <v>930</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
+      <c r="O6" s="4">
+        <v>0</v>
+      </c>
+      <c r="P6" s="4"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="4">
+        <v>512</v>
+      </c>
+      <c r="D7" s="4">
+        <v>512</v>
+      </c>
+      <c r="E7" s="4">
+        <v>200</v>
+      </c>
+      <c r="F7" s="4">
+        <v>144</v>
+      </c>
+      <c r="G7" s="4">
+        <v>174</v>
+      </c>
+      <c r="H7" s="4">
+        <v>256</v>
+      </c>
+      <c r="I7" s="4">
+        <v>256</v>
+      </c>
+      <c r="J7" s="4">
+        <v>860</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1024</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1586</v>
+      </c>
+      <c r="M7" s="4">
+        <v>606</v>
+      </c>
+      <c r="N7" s="4">
+        <v>644</v>
+      </c>
+      <c r="O7" s="4">
+        <v>1088</v>
+      </c>
+      <c r="P7" s="4"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="B8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="4">
+        <v>520</v>
+      </c>
+      <c r="D8" s="4">
+        <v>520</v>
+      </c>
+      <c r="E8" s="4">
+        <v>208</v>
+      </c>
+      <c r="F8" s="4">
+        <v>160</v>
+      </c>
+      <c r="G8" s="4">
+        <v>214</v>
+      </c>
+      <c r="H8" s="4">
+        <v>288</v>
+      </c>
+      <c r="I8" s="4">
+        <v>272</v>
+      </c>
+      <c r="J8" s="4">
+        <v>884</v>
+      </c>
+      <c r="K8" s="4">
+        <v>1058</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1983</v>
+      </c>
+      <c r="M8" s="4">
+        <v>1387</v>
+      </c>
+      <c r="N8" s="4">
+        <v>676</v>
+      </c>
+      <c r="O8" s="4">
+        <v>1158</v>
+      </c>
+      <c r="P8" s="4"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4">
+        <v>6</v>
+      </c>
+      <c r="E9" s="4">
+        <v>5</v>
+      </c>
+      <c r="F9" s="4">
+        <v>8</v>
+      </c>
+      <c r="G9" s="4">
+        <v>8</v>
+      </c>
+      <c r="H9" s="4">
+        <v>8</v>
+      </c>
+      <c r="I9" s="4">
+        <v>16</v>
+      </c>
+      <c r="J9" s="4">
+        <v>3</v>
+      </c>
+      <c r="K9" s="4">
+        <v>8</v>
+      </c>
+      <c r="L9" s="4">
+        <v>41</v>
+      </c>
+      <c r="M9" s="4">
+        <v>33</v>
+      </c>
+      <c r="N9" s="4">
+        <v>4</v>
+      </c>
+      <c r="O9" s="4">
+        <v>70</v>
+      </c>
+      <c r="P9" s="4"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="4">
+        <v>11</v>
+      </c>
+      <c r="D10" s="4">
+        <v>24</v>
+      </c>
+      <c r="E10" s="4">
+        <v>16</v>
+      </c>
+      <c r="F10" s="4">
+        <v>38</v>
+      </c>
+      <c r="G10" s="4">
+        <v>165</v>
+      </c>
+      <c r="H10" s="4">
+        <v>27</v>
+      </c>
+      <c r="I10" s="4">
+        <v>73</v>
+      </c>
+      <c r="J10" s="4">
+        <v>43</v>
+      </c>
+      <c r="K10" s="4">
+        <v>48</v>
+      </c>
+      <c r="L10" s="4">
+        <v>637</v>
+      </c>
+      <c r="M10" s="4">
+        <v>475</v>
+      </c>
+      <c r="N10" s="4">
+        <v>47</v>
+      </c>
+      <c r="O10" s="4">
+        <v>272</v>
+      </c>
+      <c r="P10" s="4"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="11">
+        <f>100*C9/C10</f>
+        <v>9.0909090909090917</v>
+      </c>
+      <c r="D11" s="11">
+        <f t="shared" ref="D11:H11" si="0">100*D9/D10</f>
+        <v>25</v>
+      </c>
+      <c r="E11" s="11">
+        <f t="shared" si="0"/>
+        <v>31.25</v>
+      </c>
+      <c r="F11" s="11">
+        <f t="shared" si="0"/>
+        <v>21.05263157894737</v>
+      </c>
+      <c r="G11" s="11">
+        <f t="shared" si="0"/>
+        <v>4.8484848484848486</v>
+      </c>
+      <c r="H11" s="11">
+        <f t="shared" si="0"/>
+        <v>29.62962962962963</v>
+      </c>
+      <c r="I11" s="11">
+        <f>100*I9/I10</f>
+        <v>21.917808219178081</v>
+      </c>
+      <c r="J11" s="11">
+        <f>100*J9/J10</f>
+        <v>6.9767441860465116</v>
+      </c>
+      <c r="K11" s="11">
+        <f>100*K9/K10</f>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="L11" s="11">
+        <f>100*L9/L10</f>
+        <v>6.4364207221350078</v>
+      </c>
+      <c r="M11" s="11">
+        <f>100*M9/M10</f>
+        <v>6.9473684210526319</v>
+      </c>
+      <c r="N11" s="11">
+        <f>100*N9/N10</f>
+        <v>8.5106382978723403</v>
+      </c>
+      <c r="O11" s="11">
+        <f>100*O9/O10</f>
+        <v>25.735294117647058</v>
+      </c>
+      <c r="P11" s="4"/>
+    </row>
+    <row r="12" spans="1:16" s="4" customFormat="1">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1.69</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1.57</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1.37</v>
+      </c>
+      <c r="I12" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="J12" s="4">
+        <v>1</v>
+      </c>
+      <c r="K12" s="4">
+        <v>1</v>
+      </c>
+      <c r="L12" s="4">
+        <v>1.08</v>
+      </c>
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
+      <c r="N12" s="4">
+        <v>1</v>
+      </c>
+      <c r="O12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="4" customFormat="1">
+      <c r="B13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>42</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>-224</v>
+      </c>
+      <c r="G13" s="4">
+        <v>-1502</v>
+      </c>
+      <c r="H13" s="4">
+        <v>-94</v>
+      </c>
+      <c r="I13" s="4">
+        <v>-20</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>48</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="4" customFormat="1">
+      <c r="A14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1.91</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1.52</v>
+      </c>
+      <c r="E14" s="4">
+        <v>6.44</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1.03</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
+      <c r="H14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
+        <v>1.03</v>
+      </c>
+      <c r="J14" s="4">
+        <v>1.23</v>
+      </c>
+      <c r="K14" s="4">
+        <v>1</v>
+      </c>
+      <c r="L14" s="4">
+        <v>2.16</v>
+      </c>
+      <c r="M14" s="4">
+        <v>1.76</v>
+      </c>
+      <c r="N14" s="4">
+        <v>1</v>
+      </c>
+      <c r="O14" s="4">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="4" customFormat="1">
+      <c r="A15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+      <c r="H15" s="4">
+        <v>1</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1</v>
+      </c>
+      <c r="J15" s="4">
+        <v>1</v>
+      </c>
+      <c r="K15" s="4">
+        <v>4.3</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1.06</v>
+      </c>
+      <c r="M15" s="4">
+        <v>1.65</v>
+      </c>
+      <c r="N15" s="4">
+        <v>1</v>
+      </c>
+      <c r="O15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+    </row>
+    <row r="18" spans="1:16" s="3" customFormat="1">
+      <c r="A18" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" t="str">
+        <f>A3</f>
+        <v>Issue</v>
+      </c>
+      <c r="B20" t="str">
+        <f>B3</f>
+        <v>Measure</v>
+      </c>
+      <c r="C20" t="str">
+        <f>C3</f>
+        <v>B.sort</v>
+      </c>
+      <c r="D20" t="str">
+        <f>D3</f>
+        <v>H.sort</v>
+      </c>
+      <c r="E20" t="str">
+        <f>E3</f>
+        <v>Bin.Search</v>
+      </c>
+      <c r="F20" t="str">
+        <f>F3</f>
+        <v>XXTEA</v>
+      </c>
+      <c r="G20" t="str">
+        <f>G3</f>
+        <v>MD5</v>
+      </c>
+      <c r="H20" t="str">
+        <f>H3</f>
+        <v>RC5</v>
+      </c>
+      <c r="I20" t="str">
+        <f>I3</f>
+        <v>FFT16</v>
+      </c>
+      <c r="J20" t="str">
+        <f>J3</f>
+        <v>Outlier</v>
+      </c>
+      <c r="K20" t="str">
+        <f>K3</f>
+        <v>LEC</v>
+      </c>
+      <c r="L20" t="str">
+        <f>L3</f>
+        <v>CoreMark</v>
+      </c>
+      <c r="M20" t="str">
+        <f>M3</f>
+        <v>MoteTrack</v>
+      </c>
+      <c r="N20" t="str">
+        <f>N3</f>
+        <v>HeatCalib</v>
+      </c>
+      <c r="O20" t="str">
+        <f>O3</f>
+        <v>HeatDetect</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" t="str">
+        <f>A4</f>
+        <v>Support for constant data</v>
+      </c>
+      <c r="B21" t="str">
+        <f>B4</f>
+        <v>Size of constant data</v>
+      </c>
+      <c r="C21" t="str">
+        <f>IF(C4&gt;0,C4,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="D21" t="str">
+        <f>IF(D4&gt;0,D4,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="E21" t="str">
+        <f>IF(E4&gt;0,E4,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="F21" t="str">
+        <f>IF(F4&gt;0,F4,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="G21" t="str">
+        <f>IF(G4&gt;0,G4,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="H21">
+        <f>IF(H4&gt;0,H4,"x")</f>
+        <v>200</v>
+      </c>
+      <c r="I21">
+        <f>IF(I4&gt;0,I4,"x")</f>
+        <v>2048</v>
+      </c>
+      <c r="J21" t="str">
+        <f>IF(J4&gt;0,J4,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="K21">
+        <f>IF(K4&gt;0,K4,"x")</f>
+        <v>51</v>
+      </c>
+      <c r="L21" t="str">
+        <f>IF(L4&gt;0,L4,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="M21" t="str">
+        <f>IF(M4&gt;0,M4,"x")</f>
+        <v>20KB</v>
+      </c>
+      <c r="N21" t="str">
+        <f>IF(N4&gt;0,N4,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="O21" t="str">
+        <f>IF(O4&gt;0,O4,"x")</f>
+        <v>x</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="B22" t="str">
+        <f>B5</f>
+        <v>Const array RAM overhead</v>
+      </c>
+      <c r="C22" t="str">
+        <f>IF(C5&gt;0,C5,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="D22" t="str">
+        <f>IF(D5&gt;0,D5,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="E22" t="str">
+        <f>IF(E5&gt;0,E5,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="F22" t="str">
+        <f>IF(F5&gt;0,F5,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="G22" t="str">
+        <f>IF(G5&gt;0,G5,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="H22">
+        <f>IF(H5&gt;0,H5,"x")</f>
+        <v>208</v>
+      </c>
+      <c r="I22" s="5">
+        <f>IF(I5&gt;0,I5,"x")</f>
+        <v>2056</v>
+      </c>
+      <c r="J22" t="str">
+        <f>IF(J5&gt;0,J5,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="K22">
+        <f>IF(K5&gt;0,K5,"x")</f>
+        <v>67</v>
+      </c>
+      <c r="L22" t="str">
+        <f>IF(L5&gt;0,L5,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="M22" s="5" t="str">
+        <f>IF(M5&gt;0,M5,"x")</f>
+        <v>too big</v>
+      </c>
+      <c r="N22" t="str">
+        <f>IF(N5&gt;0,N5,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="O22" t="str">
+        <f>IF(O5&gt;0,O5,"x")</f>
+        <v>x</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="B23" t="str">
+        <f>B6</f>
+        <v>Const array flash overhead (AOT)</v>
+      </c>
+      <c r="C23" t="str">
+        <f>IF(C6&gt;0,C6,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="D23" t="str">
+        <f>IF(D6&gt;0,D6,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="E23" t="str">
+        <f>IF(E6&gt;0,E6,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="F23" t="str">
+        <f>IF(F6&gt;0,F6,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="G23" t="str">
+        <f>IF(G6&gt;0,G6,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="H23">
+        <f>IF(H6&gt;0,H6,"x")</f>
+        <v>1998</v>
+      </c>
+      <c r="I23" s="5">
+        <f>IF(I6&gt;0,I6,"x")</f>
+        <v>26714</v>
+      </c>
+      <c r="J23" t="str">
+        <f>IF(J6&gt;0,J6,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="K23">
+        <f>IF(K6&gt;0,K6,"x")</f>
+        <v>930</v>
+      </c>
+      <c r="L23" t="str">
+        <f>IF(L6&gt;0,L6,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="M23" s="5" t="str">
+        <f>IF(M6&gt;0,M6,"x")</f>
+        <v>too big</v>
+      </c>
+      <c r="N23" t="str">
+        <f>IF(N6&gt;0,N6,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="O23" t="str">
+        <f>IF(O6&gt;0,O6,"x")</f>
+        <v>x</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" t="str">
+        <f>A7</f>
+        <v>Support for nested data structures</v>
+      </c>
+      <c r="B24" t="str">
+        <f>B7</f>
+        <v>Size of main data structures in C</v>
+      </c>
+      <c r="C24">
+        <f>C7</f>
+        <v>512</v>
+      </c>
+      <c r="D24">
+        <f>D7</f>
+        <v>512</v>
+      </c>
+      <c r="E24">
+        <f>E7</f>
+        <v>200</v>
+      </c>
+      <c r="F24">
+        <f>F7</f>
+        <v>144</v>
+      </c>
+      <c r="G24">
+        <f>G7</f>
+        <v>174</v>
+      </c>
+      <c r="H24">
+        <f>H7</f>
+        <v>256</v>
+      </c>
+      <c r="I24">
+        <f>I7</f>
+        <v>256</v>
+      </c>
+      <c r="J24">
+        <f>J7</f>
+        <v>860</v>
+      </c>
+      <c r="K24">
+        <f>K7</f>
+        <v>1024</v>
+      </c>
+      <c r="L24">
+        <f>L7</f>
+        <v>1586</v>
+      </c>
+      <c r="M24">
+        <f>M7</f>
+        <v>606</v>
+      </c>
+      <c r="N24">
+        <f>N7</f>
+        <v>644</v>
+      </c>
+      <c r="O24">
+        <f>O7</f>
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="B25" t="str">
+        <f>B8</f>
+        <v>Size of main data structures in Java</v>
+      </c>
+      <c r="C25">
+        <f>C8</f>
+        <v>520</v>
+      </c>
+      <c r="D25">
+        <f>D8</f>
+        <v>520</v>
+      </c>
+      <c r="E25">
+        <f>E8</f>
+        <v>208</v>
+      </c>
+      <c r="F25">
+        <f>F8</f>
+        <v>160</v>
+      </c>
+      <c r="G25">
+        <f>G8</f>
+        <v>214</v>
+      </c>
+      <c r="H25">
+        <f>H8</f>
+        <v>288</v>
+      </c>
+      <c r="I25">
+        <f>I8</f>
+        <v>272</v>
+      </c>
+      <c r="J25">
+        <f>J8</f>
+        <v>884</v>
+      </c>
+      <c r="K25">
+        <f>K8</f>
+        <v>1058</v>
+      </c>
+      <c r="L25">
+        <f>L8</f>
+        <v>1983</v>
+      </c>
+      <c r="M25">
+        <f>M8</f>
+        <v>1387</v>
+      </c>
+      <c r="N25">
+        <f>N8</f>
+        <v>676</v>
+      </c>
+      <c r="O25">
+        <f>O8</f>
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="8">
+        <f>C25/C24-1</f>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="D26" s="8">
+        <f t="shared" ref="D26:O26" si="1">D25/D24-1</f>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="E26" s="8">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F26" s="8">
+        <f t="shared" si="1"/>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="G26" s="8">
+        <f t="shared" si="1"/>
+        <v>0.22988505747126431</v>
+      </c>
+      <c r="H26" s="8">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+      <c r="I26" s="8">
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="J26" s="8">
+        <f t="shared" si="1"/>
+        <v>2.7906976744185963E-2</v>
+      </c>
+      <c r="K26" s="8">
+        <f t="shared" si="1"/>
+        <v>3.3203125E-2</v>
+      </c>
+      <c r="L26" s="15">
+        <f t="shared" si="1"/>
+        <v>0.25031525851197989</v>
+      </c>
+      <c r="M26" s="13">
+        <f t="shared" si="1"/>
+        <v>1.2887788778877889</v>
+      </c>
+      <c r="N26" s="8">
+        <f t="shared" si="1"/>
+        <v>4.9689440993788914E-2</v>
+      </c>
+      <c r="O26" s="8">
+        <f t="shared" si="1"/>
+        <v>6.4338235294117752E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" t="str">
+        <f>A9</f>
+        <v>Better lang. support for shorts and bytes</v>
+      </c>
+      <c r="B27" t="str">
+        <f>B9</f>
+        <v>Casts</v>
+      </c>
+      <c r="C27">
+        <f>C9</f>
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <f>D9</f>
+        <v>6</v>
+      </c>
+      <c r="E27">
+        <f>E9</f>
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <f>F9</f>
+        <v>8</v>
+      </c>
+      <c r="G27">
+        <f>G9</f>
+        <v>8</v>
+      </c>
+      <c r="H27">
+        <f>H9</f>
+        <v>8</v>
+      </c>
+      <c r="I27">
+        <f>I9</f>
+        <v>16</v>
+      </c>
+      <c r="J27">
+        <f>J9</f>
+        <v>3</v>
+      </c>
+      <c r="K27">
+        <f>K9</f>
+        <v>8</v>
+      </c>
+      <c r="L27">
+        <f>L9</f>
+        <v>41</v>
+      </c>
+      <c r="M27">
+        <f>M9</f>
+        <v>33</v>
+      </c>
+      <c r="N27">
+        <f>N9</f>
+        <v>4</v>
+      </c>
+      <c r="O27">
+        <f>O9</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="B28" t="str">
+        <f>B10</f>
+        <v>LOC</v>
+      </c>
+      <c r="C28">
+        <f>C10</f>
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <f>D10</f>
+        <v>24</v>
+      </c>
+      <c r="E28">
+        <f>E10</f>
+        <v>16</v>
+      </c>
+      <c r="F28">
+        <f>F10</f>
+        <v>38</v>
+      </c>
+      <c r="G28">
+        <f>G10</f>
+        <v>165</v>
+      </c>
+      <c r="H28">
+        <f>H10</f>
+        <v>27</v>
+      </c>
+      <c r="I28">
+        <f>I10</f>
+        <v>73</v>
+      </c>
+      <c r="J28">
+        <f>J10</f>
+        <v>43</v>
+      </c>
+      <c r="K28">
+        <f>K10</f>
+        <v>48</v>
+      </c>
+      <c r="L28">
+        <f>L10</f>
+        <v>637</v>
+      </c>
+      <c r="M28">
+        <f>M10</f>
+        <v>475</v>
+      </c>
+      <c r="N28">
+        <f>N10</f>
+        <v>47</v>
+      </c>
+      <c r="O28">
+        <f>O10</f>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="B29" t="str">
+        <f>B11</f>
+        <v>Casts per 100 LOC</v>
+      </c>
+      <c r="C29" s="6">
+        <f>C11</f>
+        <v>9.0909090909090917</v>
+      </c>
+      <c r="D29" s="7">
+        <f>D11</f>
+        <v>25</v>
+      </c>
+      <c r="E29" s="7">
+        <f>E11</f>
+        <v>31.25</v>
+      </c>
+      <c r="F29" s="6">
+        <f>F11</f>
+        <v>21.05263157894737</v>
+      </c>
+      <c r="G29" s="6">
+        <f>G11</f>
+        <v>4.8484848484848486</v>
+      </c>
+      <c r="H29" s="7">
+        <f>H11</f>
+        <v>29.62962962962963</v>
+      </c>
+      <c r="I29" s="6">
+        <f>I11</f>
+        <v>21.917808219178081</v>
+      </c>
+      <c r="J29" s="6">
+        <f>J11</f>
+        <v>6.9767441860465116</v>
+      </c>
+      <c r="K29" s="6">
+        <f>K11</f>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="L29" s="6">
+        <f>L11</f>
+        <v>6.4364207221350078</v>
+      </c>
+      <c r="M29" s="6">
+        <f>M11</f>
+        <v>6.9473684210526319</v>
+      </c>
+      <c r="N29" s="6">
+        <f>N11</f>
+        <v>8.5106382978723403</v>
+      </c>
+      <c r="O29" s="7">
+        <f>O11</f>
+        <v>25.735294117647058</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" t="str">
+        <f>A12</f>
+        <v>Explicit and efficient inlining</v>
+      </c>
+      <c r="B30" t="str">
+        <f>B12</f>
+        <v>Slowdown non-inlined version</v>
+      </c>
+      <c r="C30" s="9" t="str">
+        <f>IF(C12&gt;1,C12-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="D30" s="12">
+        <f>IF(D12&gt;1,D12-1,"x")</f>
+        <v>0.69</v>
+      </c>
+      <c r="E30" s="9" t="str">
+        <f>IF(E12&gt;1,E12-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="F30" s="12">
+        <f>IF(F12&gt;1,F12-1,"x")</f>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="G30" s="9">
+        <f>IF(G12&gt;1,G12-1,"x")</f>
+        <v>0.25</v>
+      </c>
+      <c r="H30" s="9">
+        <f>IF(H12&gt;1,H12-1,"x")</f>
+        <v>0.37000000000000011</v>
+      </c>
+      <c r="I30" s="9">
+        <f>IF(I12&gt;1,I12-1,"x")</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="J30" s="9" t="str">
+        <f>IF(J12&gt;1,J12-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="K30" s="9" t="str">
+        <f>IF(K12&gt;1,K12-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="L30" s="9">
+        <f>IF(L12&gt;1,L12-1,"x")</f>
+        <v>8.0000000000000071E-2</v>
+      </c>
+      <c r="M30" s="9" t="str">
+        <f>IF(M12&gt;1,M12-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="N30" s="9" t="str">
+        <f>IF(N12&gt;1,N12-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="O30" s="9" t="str">
+        <f>IF(O12&gt;1,O12-1,"x")</f>
+        <v>x</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="B31" t="str">
+        <f>B13</f>
+        <v>Size non-inlined version</v>
+      </c>
+      <c r="C31" t="str">
+        <f>IF(C13=0,"x",C13)</f>
+        <v>x</v>
+      </c>
+      <c r="D31" s="5">
+        <f>IF(D13=0,"x",D13)</f>
+        <v>42</v>
+      </c>
+      <c r="E31" t="str">
+        <f>IF(E13=0,"x",E13)</f>
+        <v>x</v>
+      </c>
+      <c r="F31">
+        <f>IF(F13=0,"x",F13)</f>
+        <v>-224</v>
+      </c>
+      <c r="G31">
+        <f>IF(G13=0,"x",G13)</f>
+        <v>-1502</v>
+      </c>
+      <c r="H31">
+        <f>IF(H13=0,"x",H13)</f>
+        <v>-94</v>
+      </c>
+      <c r="I31">
+        <f>IF(I13=0,"x",I13)</f>
+        <v>-20</v>
+      </c>
+      <c r="J31" t="str">
+        <f>IF(J13=0,"x",J13)</f>
+        <v>x</v>
+      </c>
+      <c r="K31" t="str">
+        <f>IF(K13=0,"x",K13)</f>
+        <v>x</v>
+      </c>
+      <c r="L31" s="5">
+        <f>IF(L13=0,"x",L13)</f>
+        <v>48</v>
+      </c>
+      <c r="M31" t="str">
+        <f>IF(M13=0,"x",M13)</f>
+        <v>x</v>
+      </c>
+      <c r="N31" t="str">
+        <f>IF(N13=0,"x",N13)</f>
+        <v>x</v>
+      </c>
+      <c r="O31" t="str">
+        <f>IF(O13=0,"x",O13)</f>
+        <v>x</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" t="str">
+        <f>A14</f>
+        <v>An optimising compiler</v>
+      </c>
+      <c r="B32" t="str">
+        <f>B14</f>
+        <v>Slowdown w/o optimisations</v>
+      </c>
+      <c r="C32" s="12">
+        <f>IF(C14&gt;1,C14-1,"x")</f>
+        <v>0.90999999999999992</v>
+      </c>
+      <c r="D32" s="12">
+        <f>IF(D14&gt;1,D14-1,"x")</f>
+        <v>0.52</v>
+      </c>
+      <c r="E32" s="12">
+        <f>IF(E14&gt;1,E14-1,"x")</f>
+        <v>5.44</v>
+      </c>
+      <c r="F32" s="9">
+        <f>IF(F14&gt;1,F14-1,"x")</f>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="G32" s="9" t="str">
+        <f>IF(G14&gt;1,G14-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="H32" s="9" t="str">
+        <f>IF(H14&gt;1,H14-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="I32" s="9">
+        <f>IF(I14&gt;1,I14-1,"x")</f>
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="J32" s="9">
+        <f>IF(J14&gt;1,J14-1,"x")</f>
+        <v>0.22999999999999998</v>
+      </c>
+      <c r="K32" s="9" t="str">
+        <f>IF(K14&gt;1,K14-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="L32" s="12">
+        <f>IF(L14&gt;1,L14-1,"x")</f>
+        <v>1.1600000000000001</v>
+      </c>
+      <c r="M32" s="12">
+        <f>IF(M14&gt;1,M14-1,"x")</f>
+        <v>0.76</v>
+      </c>
+      <c r="N32" s="9" t="str">
+        <f>IF(N14&gt;1,N14-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="O32" s="9">
+        <f>IF(O14&gt;1,O14-1,"x")</f>
+        <v>2.0000000000000018E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" t="str">
+        <f>A15</f>
+        <v>Allocating objects on stack</v>
+      </c>
+      <c r="B33" t="str">
+        <f>B15</f>
+        <v>Slowdown heap allocation</v>
+      </c>
+      <c r="C33" s="9" t="str">
+        <f>IF(C15&gt;1,C15-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="D33" s="9" t="str">
+        <f>IF(D15&gt;1,D15-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="E33" s="9" t="str">
+        <f>IF(E15&gt;1,E15-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="F33" s="9" t="str">
+        <f>IF(F15&gt;1,F15-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="G33" s="9" t="str">
+        <f>IF(G15&gt;1,G15-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="H33" s="9" t="str">
+        <f>IF(H15&gt;1,H15-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="I33" s="9" t="str">
+        <f>IF(I15&gt;1,I15-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="J33" s="9" t="str">
+        <f>IF(J15&gt;1,J15-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="K33" s="12">
+        <f>IF(K15&gt;1,K15-1,"x")</f>
+        <v>3.3</v>
+      </c>
+      <c r="L33" s="9">
+        <f>IF(L15&gt;1,L15-1,"x")</f>
+        <v>6.0000000000000053E-2</v>
+      </c>
+      <c r="M33" s="12">
+        <f>IF(M15&gt;1,M15-1,"x")</f>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="N33" s="9" t="str">
+        <f>IF(N15&gt;1,N15-1,"x")</f>
+        <v>x</v>
+      </c>
+      <c r="O33" s="9" t="str">
+        <f>IF(O15&gt;1,O15-1,"x")</f>
+        <v>x</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="E36" s="1"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Comments prof Shih Chapter 4
</commit_message>
<xml_diff>
--- a/data/java-issues-quantitative-results.xlsx
+++ b/data/java-issues-quantitative-results.xlsx
@@ -207,8 +207,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="119">
+  <cellStyleXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -346,7 +348,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="119">
+  <cellStyles count="121">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -406,6 +408,7 @@
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -465,6 +468,7 @@
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2024,7 +2028,7 @@
   <dimension ref="A3:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2256,7 +2260,7 @@
         <v>1024</v>
       </c>
       <c r="L7" s="4">
-        <v>1586</v>
+        <v>1633</v>
       </c>
       <c r="M7" s="4">
         <v>606</v>
@@ -2980,7 +2984,7 @@
       </c>
       <c r="L24">
         <f>L7</f>
-        <v>1586</v>
+        <v>1633</v>
       </c>
       <c r="M24">
         <f>M7</f>
@@ -3095,7 +3099,7 @@
       </c>
       <c r="L26" s="15">
         <f t="shared" si="1"/>
-        <v>0.25031525851197989</v>
+        <v>0.21432945499081435</v>
       </c>
       <c r="M26" s="13">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
All \items with a capital, make sure issues tbl is consistnt with source
</commit_message>
<xml_diff>
--- a/data/java-issues-quantitative-results.xlsx
+++ b/data/java-issues-quantitative-results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31200" windowHeight="18780" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data for all bm" sheetId="2" r:id="rId1"/>
@@ -2042,7 +2042,7 @@
   <dimension ref="A3:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2364,7 +2364,7 @@
         <v>3</v>
       </c>
       <c r="K9" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L9" s="4">
         <v>70</v>
@@ -2376,7 +2376,7 @@
         <v>4</v>
       </c>
       <c r="O9" s="4">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="P9" s="4"/>
     </row>
@@ -2407,10 +2407,10 @@
         <v>73</v>
       </c>
       <c r="J10" s="4">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K10" s="4">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="L10" s="4">
         <v>849</v>
@@ -2419,10 +2419,10 @@
         <v>475</v>
       </c>
       <c r="N10" s="4">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="O10" s="4">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="P10" s="4"/>
     </row>
@@ -2461,11 +2461,11 @@
       </c>
       <c r="J11" s="11">
         <f t="shared" si="1"/>
-        <v>6.9767441860465116</v>
+        <v>6.8181818181818183</v>
       </c>
       <c r="K11" s="11">
         <f t="shared" si="1"/>
-        <v>16.666666666666668</v>
+        <v>12.987012987012987</v>
       </c>
       <c r="L11" s="11">
         <f t="shared" si="1"/>
@@ -2477,11 +2477,11 @@
       </c>
       <c r="N11" s="11">
         <f t="shared" si="1"/>
-        <v>8.5106382978723403</v>
+        <v>7.8431372549019605</v>
       </c>
       <c r="O11" s="11">
         <f t="shared" si="1"/>
-        <v>25.735294117647058</v>
+        <v>24.060150375939848</v>
       </c>
       <c r="P11" s="4"/>
     </row>
@@ -3171,7 +3171,7 @@
       </c>
       <c r="K27">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L27">
         <f t="shared" si="9"/>
@@ -3187,7 +3187,7 @@
       </c>
       <c r="O27">
         <f t="shared" si="9"/>
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -3225,11 +3225,11 @@
       </c>
       <c r="J28">
         <f t="shared" si="10"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K28">
         <f t="shared" si="10"/>
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="L28">
         <f t="shared" si="10"/>
@@ -3241,11 +3241,11 @@
       </c>
       <c r="N28">
         <f t="shared" si="10"/>
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="O28">
         <f t="shared" si="10"/>
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -3283,11 +3283,11 @@
       </c>
       <c r="J29" s="6">
         <f t="shared" si="11"/>
-        <v>6.9767441860465116</v>
+        <v>6.8181818181818183</v>
       </c>
       <c r="K29" s="6">
         <f t="shared" si="11"/>
-        <v>16.666666666666668</v>
+        <v>12.987012987012987</v>
       </c>
       <c r="L29" s="6">
         <f t="shared" si="11"/>
@@ -3299,11 +3299,11 @@
       </c>
       <c r="N29" s="6">
         <f t="shared" si="11"/>
-        <v>8.5106382978723403</v>
+        <v>7.8431372549019605</v>
       </c>
       <c r="O29" s="7">
         <f t="shared" si="11"/>
-        <v>25.735294117647058</v>
+        <v>24.060150375939848</v>
       </c>
     </row>
     <row r="30" spans="1:16">

</xml_diff>